<commit_message>
Atualizaçao da tabela RVND x RVND2
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/RVND x RVND2.xlsx
+++ b/Arquivos/Comparações/RVND x RVND2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="73">
   <si>
     <t>Comparação entre as duas versões do RVND</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>att532</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>bayg29</t>
@@ -237,22 +240,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0_ "/>
     <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -280,7 +276,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -296,32 +291,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,73 +301,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,7 +315,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,6 +369,52 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -433,13 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,7 +441,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,67 +483,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,55 +507,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,7 +525,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +543,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,20 +653,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,26 +675,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,22 +718,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,152 +753,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -915,34 +911,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1266,8 +1256,8 @@
   <sheetPr/>
   <dimension ref="B2:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1367,7 +1357,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="6">
-        <v>617.02</v>
+        <v>610</v>
       </c>
       <c r="E4" s="7">
         <v>609.06</v>
@@ -1382,10 +1372,10 @@
       <c r="I4" s="5">
         <v>140</v>
       </c>
-      <c r="J4" s="6">
-        <v>1293.78</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="J4" s="9">
+        <v>1289.37</v>
+      </c>
+      <c r="K4" s="6">
         <v>1286.16</v>
       </c>
       <c r="L4" s="4" t="str">
@@ -1395,16 +1385,16 @@
       <c r="N4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <v>210</v>
       </c>
-      <c r="P4" s="12">
-        <v>1988.64</v>
-      </c>
-      <c r="Q4" s="9">
+      <c r="P4" s="9">
+        <v>1933.85</v>
+      </c>
+      <c r="Q4" s="6">
         <v>1925.22</v>
       </c>
-      <c r="R4" s="13" t="str">
+      <c r="R4" s="11" t="str">
         <f>IF(P4&lt;Q4,"RVND2",IF(Q4&lt;P4,"RVND","Igual"))</f>
         <v>RVND</v>
       </c>
@@ -1417,14 +1407,14 @@
         <v>12</v>
       </c>
       <c r="D5" s="6">
-        <v>1373</v>
+        <v>1239</v>
       </c>
       <c r="E5" s="7">
         <v>1239</v>
       </c>
       <c r="F5" s="4" t="str">
         <f t="shared" ref="F5:F36" si="0">IF(D5&lt;E5,"RVND2",IF(E5&lt;D5,"RVND","Igual"))</f>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>7</v>
@@ -1432,10 +1422,10 @@
       <c r="I5" s="5">
         <v>24</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="9">
         <v>3231</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="6">
         <v>3231</v>
       </c>
       <c r="L5" s="4" t="str">
@@ -1445,18 +1435,18 @@
       <c r="N5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <v>36</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="9">
+        <v>6252</v>
+      </c>
+      <c r="Q5" s="6">
         <v>6348</v>
       </c>
-      <c r="Q5" s="9">
-        <v>6348</v>
-      </c>
-      <c r="R5" s="13" t="str">
+      <c r="R5" s="11" t="str">
         <f t="shared" ref="R5:R36" si="2">IF(P5&lt;Q5,"RVND2",IF(Q5&lt;P5,"RVND","Igual"))</f>
-        <v>Igual</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="2:18">
@@ -1467,14 +1457,14 @@
         <v>133</v>
       </c>
       <c r="D6" s="6">
-        <v>5470</v>
+        <v>5254</v>
       </c>
       <c r="E6" s="7">
         <v>5348</v>
       </c>
       <c r="F6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>8</v>
@@ -1482,60 +1472,59 @@
       <c r="I6" s="5">
         <v>266</v>
       </c>
-      <c r="J6" s="6">
-        <v>13957</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="J6" s="9">
+        <v>11954</v>
+      </c>
+      <c r="K6" s="6">
         <v>11954</v>
       </c>
       <c r="L6" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="10">
         <v>399</v>
       </c>
-      <c r="P6" s="12">
-        <v>21371</v>
-      </c>
-      <c r="Q6" s="9">
+      <c r="P6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="6">
         <v>18238</v>
       </c>
-      <c r="R6" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>RVND</v>
+      <c r="R6" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="2:18">
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5">
         <v>7</v>
       </c>
       <c r="D7" s="6">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="E7" s="7">
         <v>275</v>
       </c>
       <c r="F7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7" s="5">
         <v>14</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="9">
         <v>581</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="6">
         <v>581</v>
       </c>
       <c r="L7" s="4" t="str">
@@ -1543,99 +1532,99 @@
         <v>Igual</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="11">
+        <v>10</v>
+      </c>
+      <c r="O7" s="10">
         <v>21</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="9">
         <v>1035</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="6">
         <v>1035</v>
       </c>
-      <c r="R7" s="13" t="str">
+      <c r="R7" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Igual</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="2:18">
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
       </c>
       <c r="D8" s="6">
-        <v>352</v>
+        <v>319</v>
       </c>
       <c r="E8" s="7">
         <v>319</v>
       </c>
       <c r="F8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I8" s="5">
         <v>14</v>
       </c>
-      <c r="J8" s="6">
-        <v>816</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="J8" s="9">
+        <v>651</v>
+      </c>
+      <c r="K8" s="6">
         <v>692</v>
       </c>
       <c r="L8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="11">
+        <v>11</v>
+      </c>
+      <c r="O8" s="10">
         <v>21</v>
       </c>
-      <c r="P8" s="12">
-        <v>1218</v>
-      </c>
-      <c r="Q8" s="9">
+      <c r="P8" s="9">
+        <v>1159</v>
+      </c>
+      <c r="Q8" s="6">
         <v>1128</v>
       </c>
-      <c r="R8" s="13" t="str">
+      <c r="R8" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="2:18">
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5">
         <v>13</v>
       </c>
       <c r="D9" s="6">
-        <v>556.81</v>
+        <v>480.48</v>
       </c>
       <c r="E9" s="7">
         <v>480.48</v>
       </c>
       <c r="F9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" s="5">
         <v>26</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="9">
         <v>1766.5</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="6">
         <v>1766.5</v>
       </c>
       <c r="L9" s="4" t="str">
@@ -1643,31 +1632,31 @@
         <v>Igual</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="11">
+        <v>12</v>
+      </c>
+      <c r="O9" s="10">
         <v>39</v>
       </c>
-      <c r="P9" s="12">
-        <v>4246.84</v>
-      </c>
-      <c r="Q9" s="9">
+      <c r="P9" s="9">
+        <v>4201.16</v>
+      </c>
+      <c r="Q9" s="6">
         <v>3910.64</v>
       </c>
-      <c r="R9" s="13" t="str">
+      <c r="R9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="2:18">
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="5">
         <v>31</v>
       </c>
       <c r="D10" s="6">
-        <v>14272.3</v>
+        <v>13213.67</v>
       </c>
       <c r="E10" s="7">
         <v>11667.28</v>
@@ -1677,15 +1666,15 @@
         <v>RVND</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" s="5">
         <v>63</v>
       </c>
-      <c r="J10" s="6">
-        <v>27710.3</v>
-      </c>
-      <c r="K10" s="9">
+      <c r="J10" s="9">
+        <v>27823.92</v>
+      </c>
+      <c r="K10" s="6">
         <v>27397.27</v>
       </c>
       <c r="L10" s="4" t="str">
@@ -1693,49 +1682,49 @@
         <v>RVND</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="11">
+        <v>13</v>
+      </c>
+      <c r="O10" s="10">
         <v>95</v>
       </c>
-      <c r="P10" s="12">
-        <v>54266.9</v>
-      </c>
-      <c r="Q10" s="9">
+      <c r="P10" s="9">
+        <v>51428.56</v>
+      </c>
+      <c r="Q10" s="6">
         <v>49142.24</v>
       </c>
-      <c r="R10" s="13" t="str">
+      <c r="R10" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:18">
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="5">
         <v>14</v>
       </c>
       <c r="D11" s="6">
-        <v>5291</v>
+        <v>4077</v>
       </c>
       <c r="E11" s="7">
         <v>4129</v>
       </c>
       <c r="F11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" s="5">
         <v>29</v>
       </c>
-      <c r="J11" s="6">
-        <v>10262</v>
-      </c>
-      <c r="K11" s="9">
+      <c r="J11" s="9">
+        <v>6939</v>
+      </c>
+      <c r="K11" s="6">
         <v>6805</v>
       </c>
       <c r="L11" s="4" t="str">
@@ -1743,25 +1732,25 @@
         <v>RVND</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="11">
+        <v>14</v>
+      </c>
+      <c r="O11" s="10">
         <v>43</v>
       </c>
-      <c r="P11" s="12">
-        <v>13054</v>
-      </c>
-      <c r="Q11" s="9">
+      <c r="P11" s="9">
+        <v>10708</v>
+      </c>
+      <c r="Q11" s="6">
         <v>10285</v>
       </c>
-      <c r="R11" s="13" t="str">
+      <c r="R11" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="2:18">
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5">
         <v>45</v>
@@ -1777,15 +1766,15 @@
         <v>Igual</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="5">
         <v>90</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="9">
         <v>950</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="6">
         <v>950</v>
       </c>
       <c r="L12" s="4" t="str">
@@ -1793,25 +1782,25 @@
         <v>Igual</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="11">
+        <v>15</v>
+      </c>
+      <c r="O12" s="10">
         <v>135</v>
       </c>
-      <c r="P12" s="12">
-        <v>1480</v>
-      </c>
-      <c r="Q12" s="9">
+      <c r="P12" s="9">
         <v>1460</v>
       </c>
-      <c r="R12" s="13" t="str">
+      <c r="Q12" s="6">
+        <v>1460</v>
+      </c>
+      <c r="R12" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="2:18">
       <c r="B13" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -1827,115 +1816,115 @@
         <v>Igual</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I13" s="5">
         <v>7</v>
       </c>
-      <c r="J13" s="6">
-        <v>1454.84</v>
-      </c>
-      <c r="K13" s="9">
+      <c r="J13" s="9">
+        <v>966.37</v>
+      </c>
+      <c r="K13" s="6">
         <v>1140.19</v>
       </c>
       <c r="L13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="11">
+        <v>16</v>
+      </c>
+      <c r="O13" s="10">
         <v>10</v>
       </c>
-      <c r="P13" s="12">
-        <v>1943.98</v>
-      </c>
-      <c r="Q13" s="9">
+      <c r="P13" s="9">
         <v>1637.31</v>
       </c>
-      <c r="R13" s="13" t="str">
+      <c r="Q13" s="6">
+        <v>1637.31</v>
+      </c>
+      <c r="R13" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="2:18">
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5">
         <v>32</v>
       </c>
       <c r="D14" s="6">
-        <v>1205.2</v>
+        <v>1171.54</v>
       </c>
       <c r="E14" s="7">
         <v>1178.35</v>
       </c>
       <c r="F14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="5">
         <v>65</v>
       </c>
-      <c r="J14" s="6">
-        <v>2708.24</v>
-      </c>
-      <c r="K14" s="9">
+      <c r="J14" s="9">
+        <v>2541.67</v>
+      </c>
+      <c r="K14" s="6">
         <v>2541.67</v>
       </c>
       <c r="L14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O14" s="11">
+        <v>17</v>
+      </c>
+      <c r="O14" s="10">
         <v>97</v>
       </c>
-      <c r="P14" s="12">
-        <v>4139.55</v>
-      </c>
-      <c r="Q14" s="9">
+      <c r="P14" s="9">
         <v>3908.11</v>
       </c>
-      <c r="R14" s="13" t="str">
+      <c r="Q14" s="6">
+        <v>3908.11</v>
+      </c>
+      <c r="R14" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="2:18">
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5">
         <v>37</v>
       </c>
       <c r="D15" s="6">
-        <v>1304.57</v>
+        <v>1284.47</v>
       </c>
       <c r="E15" s="7">
         <v>1284.47</v>
       </c>
       <c r="F15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I15" s="5">
         <v>75</v>
       </c>
-      <c r="J15" s="6">
-        <v>3083.54</v>
-      </c>
-      <c r="K15" s="9">
+      <c r="J15" s="9">
+        <v>2929.1</v>
+      </c>
+      <c r="K15" s="6">
         <v>2907.65</v>
       </c>
       <c r="L15" s="4" t="str">
@@ -1943,49 +1932,49 @@
         <v>RVND</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O15" s="11">
+        <v>18</v>
+      </c>
+      <c r="O15" s="10">
         <v>112</v>
       </c>
-      <c r="P15" s="12">
-        <v>4735.37</v>
-      </c>
-      <c r="Q15" s="9">
+      <c r="P15" s="9">
+        <v>4698.48</v>
+      </c>
+      <c r="Q15" s="6">
         <v>4684.6</v>
       </c>
-      <c r="R15" s="13" t="str">
+      <c r="R15" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="2:18">
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="5">
         <v>10</v>
       </c>
       <c r="D16" s="6">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="7">
         <v>99</v>
       </c>
       <c r="F16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I16" s="5">
         <v>21</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="9">
         <v>239</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="6">
         <v>239</v>
       </c>
       <c r="L16" s="4" t="str">
@@ -1993,25 +1982,25 @@
         <v>Igual</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O16" s="11">
+        <v>19</v>
+      </c>
+      <c r="O16" s="10">
         <v>31</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="9">
         <v>413</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q16" s="6">
         <v>401</v>
       </c>
-      <c r="R16" s="13" t="str">
+      <c r="R16" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="2:18">
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5">
         <v>12</v>
@@ -2019,21 +2008,23 @@
       <c r="D17" s="6">
         <v>77.04</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="F17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I17" s="5">
         <v>25</v>
       </c>
-      <c r="J17" s="6">
-        <v>181.41</v>
-      </c>
-      <c r="K17" s="9">
+      <c r="J17" s="9">
+        <v>170.06</v>
+      </c>
+      <c r="K17" s="6">
         <v>168.63</v>
       </c>
       <c r="L17" s="4" t="str">
@@ -2041,49 +2032,49 @@
         <v>RVND</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="11">
+        <v>20</v>
+      </c>
+      <c r="O17" s="10">
         <v>38</v>
       </c>
-      <c r="P17" s="12">
-        <v>291.59</v>
-      </c>
-      <c r="Q17" s="9">
+      <c r="P17" s="9">
+        <v>282.83</v>
+      </c>
+      <c r="Q17" s="6">
         <v>281.61</v>
       </c>
-      <c r="R17" s="13" t="str">
+      <c r="R17" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="18" ht="15.75" spans="2:18">
       <c r="B18" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5">
         <v>19</v>
       </c>
       <c r="D18" s="6">
-        <v>97.38</v>
+        <v>97.21</v>
       </c>
       <c r="E18" s="7">
         <v>97.21</v>
       </c>
       <c r="F18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I18" s="5">
         <v>38</v>
       </c>
-      <c r="J18" s="6">
-        <v>229.64</v>
-      </c>
-      <c r="K18" s="9">
+      <c r="J18" s="9">
+        <v>224.62</v>
+      </c>
+      <c r="K18" s="6">
         <v>221.22</v>
       </c>
       <c r="L18" s="4" t="str">
@@ -2091,49 +2082,49 @@
         <v>RVND</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O18" s="11">
+        <v>21</v>
+      </c>
+      <c r="O18" s="10">
         <v>57</v>
       </c>
-      <c r="P18" s="12">
-        <v>343.29</v>
-      </c>
-      <c r="Q18" s="9">
+      <c r="P18" s="9">
         <v>340.02</v>
       </c>
-      <c r="R18" s="13" t="str">
+      <c r="Q18" s="6">
+        <v>340.02</v>
+      </c>
+      <c r="R18" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="2:18">
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5">
         <v>25</v>
       </c>
       <c r="D19" s="6">
-        <v>150.4</v>
+        <v>129.13</v>
       </c>
       <c r="E19" s="7">
         <v>138.13</v>
       </c>
       <c r="F19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I19" s="5">
         <v>50</v>
       </c>
-      <c r="J19" s="6">
-        <v>314.43</v>
-      </c>
-      <c r="K19" s="9">
+      <c r="J19" s="9">
+        <v>304.77</v>
+      </c>
+      <c r="K19" s="6">
         <v>286.97</v>
       </c>
       <c r="L19" s="4" t="str">
@@ -2141,81 +2132,81 @@
         <v>RVND</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="11">
+        <v>22</v>
+      </c>
+      <c r="O19" s="10">
         <v>75</v>
       </c>
-      <c r="P19" s="12">
-        <v>452.51</v>
-      </c>
-      <c r="Q19" s="9">
+      <c r="P19" s="9">
+        <v>439.3</v>
+      </c>
+      <c r="Q19" s="6">
         <v>438.75</v>
       </c>
-      <c r="R19" s="13" t="str">
+      <c r="R19" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="2:18">
       <c r="B20" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5">
         <v>6</v>
       </c>
       <c r="D20" s="6">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E20" s="7">
         <v>145</v>
       </c>
       <c r="F20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20" s="5">
         <v>13</v>
       </c>
-      <c r="J20" s="6">
-        <v>331</v>
-      </c>
-      <c r="K20" s="9">
+      <c r="J20" s="9">
+        <v>317</v>
+      </c>
+      <c r="K20" s="6">
         <v>317</v>
       </c>
       <c r="L20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="11">
+        <v>23</v>
+      </c>
+      <c r="O20" s="10">
         <v>19</v>
       </c>
-      <c r="P20" s="12">
-        <v>602</v>
-      </c>
-      <c r="Q20" s="9">
+      <c r="P20" s="9">
+        <v>495</v>
+      </c>
+      <c r="Q20" s="6">
         <v>599</v>
       </c>
-      <c r="R20" s="13" t="str">
+      <c r="R20" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="2:18">
       <c r="B21" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5">
         <v>65</v>
       </c>
       <c r="D21" s="6">
-        <v>559.01</v>
+        <v>543.96</v>
       </c>
       <c r="E21" s="7">
         <v>540.34</v>
@@ -2225,15 +2216,15 @@
         <v>RVND</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I21" s="5">
         <v>131</v>
       </c>
-      <c r="J21" s="6">
-        <v>1166.89</v>
-      </c>
-      <c r="K21" s="9">
+      <c r="J21" s="9">
+        <v>1122.23</v>
+      </c>
+      <c r="K21" s="6">
         <v>1100.26</v>
       </c>
       <c r="L21" s="4" t="str">
@@ -2241,49 +2232,49 @@
         <v>RVND</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" s="11">
+        <v>24</v>
+      </c>
+      <c r="O21" s="10">
         <v>196</v>
       </c>
-      <c r="P21" s="12">
-        <v>1702.23</v>
-      </c>
-      <c r="Q21" s="9">
+      <c r="P21" s="9">
+        <v>1650.6</v>
+      </c>
+      <c r="Q21" s="6">
         <v>1640.39</v>
       </c>
-      <c r="R21" s="13" t="str">
+      <c r="R21" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="22" ht="15.75" spans="2:18">
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
       </c>
       <c r="D22" s="6">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E22" s="7">
         <v>154</v>
       </c>
       <c r="F22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND2</v>
+        <v>Igual</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I22" s="5">
         <v>8</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="9">
         <v>359</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="6">
         <v>359</v>
       </c>
       <c r="L22" s="4" t="str">
@@ -2291,75 +2282,75 @@
         <v>Igual</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="O22" s="11">
+        <v>25</v>
+      </c>
+      <c r="O22" s="10">
         <v>12</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="9">
         <v>640</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="Q22" s="6">
         <v>640</v>
       </c>
-      <c r="R22" s="13" t="str">
+      <c r="R22" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Igual</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="2:18">
       <c r="B23" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="5">
         <v>5</v>
       </c>
       <c r="D23" s="6">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="E23" s="7">
         <v>181</v>
       </c>
       <c r="F23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
       </c>
-      <c r="J23" s="6">
-        <v>989</v>
-      </c>
-      <c r="K23" s="9">
+      <c r="J23" s="9">
+        <v>683</v>
+      </c>
+      <c r="K23" s="6">
         <v>711</v>
       </c>
       <c r="L23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" s="11">
+        <v>26</v>
+      </c>
+      <c r="O23" s="10">
         <v>15</v>
       </c>
-      <c r="P23" s="12">
-        <v>1573</v>
-      </c>
-      <c r="Q23" s="9">
+      <c r="P23" s="9">
         <v>1331</v>
       </c>
-      <c r="R23" s="13" t="str">
+      <c r="Q23" s="6">
+        <v>1331</v>
+      </c>
+      <c r="R23" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="2:18">
       <c r="B24" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="5">
         <v>6</v>
@@ -2375,15 +2366,15 @@
         <v>Igual</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I24" s="5">
         <v>12</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="9">
         <v>490</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="6">
         <v>413</v>
       </c>
       <c r="L24" s="4" t="str">
@@ -2391,25 +2382,25 @@
         <v>RVND</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O24" s="11">
+        <v>27</v>
+      </c>
+      <c r="O24" s="10">
         <v>18</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="9">
         <v>794</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q24" s="6">
         <v>794</v>
       </c>
-      <c r="R24" s="13" t="str">
+      <c r="R24" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Igual</v>
       </c>
     </row>
     <row r="25" ht="15.75" spans="2:18">
       <c r="B25" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5">
         <v>12</v>
@@ -2425,15 +2416,15 @@
         <v>RVND</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I25" s="5">
         <v>24</v>
       </c>
-      <c r="J25" s="6">
-        <v>2011</v>
-      </c>
-      <c r="K25" s="9">
+      <c r="J25" s="9">
+        <v>1719</v>
+      </c>
+      <c r="K25" s="6">
         <v>1705</v>
       </c>
       <c r="L25" s="4" t="str">
@@ -2441,81 +2432,81 @@
         <v>RVND</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="11">
+        <v>28</v>
+      </c>
+      <c r="O25" s="10">
         <v>36</v>
       </c>
-      <c r="P25" s="12">
-        <v>3164</v>
-      </c>
-      <c r="Q25" s="9">
+      <c r="P25" s="9">
         <v>3054</v>
       </c>
-      <c r="R25" s="13" t="str">
+      <c r="Q25" s="6">
+        <v>3054</v>
+      </c>
+      <c r="R25" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="2:18">
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="5">
         <v>24</v>
       </c>
       <c r="D26" s="6">
-        <v>9578.71</v>
+        <v>9332.77</v>
       </c>
       <c r="E26" s="7">
         <v>9332.77</v>
       </c>
       <c r="F26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I26" s="5">
         <v>48</v>
       </c>
-      <c r="J26" s="6">
-        <v>21055.45</v>
-      </c>
-      <c r="K26" s="9">
+      <c r="J26" s="9">
+        <v>20400.19</v>
+      </c>
+      <c r="K26" s="6">
         <v>20435.51</v>
       </c>
       <c r="L26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="11">
+        <v>29</v>
+      </c>
+      <c r="O26" s="10">
         <v>72</v>
       </c>
-      <c r="P26" s="12">
-        <v>39556.93</v>
-      </c>
-      <c r="Q26" s="9">
+      <c r="P26" s="9">
+        <v>36835.84</v>
+      </c>
+      <c r="Q26" s="6">
         <v>36699.98</v>
       </c>
-      <c r="R26" s="13" t="str">
+      <c r="R26" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="27" ht="15.75" spans="2:18">
       <c r="B27" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5">
         <v>30</v>
       </c>
       <c r="D27" s="6">
-        <v>1376</v>
+        <v>1355</v>
       </c>
       <c r="E27" s="7">
         <v>1349</v>
@@ -2525,15 +2516,15 @@
         <v>RVND</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I27" s="5">
         <v>60</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="9">
         <v>3120</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="6">
         <v>3091</v>
       </c>
       <c r="L27" s="4" t="str">
@@ -2541,25 +2532,25 @@
         <v>RVND</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="O27" s="11">
+        <v>30</v>
+      </c>
+      <c r="O27" s="10">
         <v>90</v>
       </c>
-      <c r="P27" s="12">
-        <v>4615</v>
-      </c>
-      <c r="Q27" s="9">
+      <c r="P27" s="9">
+        <v>4542</v>
+      </c>
+      <c r="Q27" s="6">
         <v>4537</v>
       </c>
-      <c r="R27" s="13" t="str">
+      <c r="R27" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="28" ht="15.75" spans="2:18">
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" s="5">
         <v>12</v>
@@ -2575,47 +2566,47 @@
         <v>Igual</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I28" s="5">
         <v>24</v>
       </c>
-      <c r="J28" s="6">
-        <v>5848</v>
-      </c>
-      <c r="K28" s="9">
+      <c r="J28" s="9">
+        <v>5398</v>
+      </c>
+      <c r="K28" s="6">
         <v>5511</v>
       </c>
       <c r="L28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="O28" s="11">
+        <v>31</v>
+      </c>
+      <c r="O28" s="10">
         <v>36</v>
       </c>
-      <c r="P28" s="12">
-        <v>8308</v>
-      </c>
-      <c r="Q28" s="9">
+      <c r="P28" s="9">
+        <v>7770</v>
+      </c>
+      <c r="Q28" s="6">
         <v>7612</v>
       </c>
-      <c r="R28" s="13" t="str">
+      <c r="R28" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="29" ht="15.75" spans="2:18">
       <c r="B29" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29" s="5">
         <v>25</v>
       </c>
       <c r="D29" s="6">
-        <v>5015.02</v>
+        <v>4739.94</v>
       </c>
       <c r="E29" s="7">
         <v>4649.79</v>
@@ -2625,65 +2616,65 @@
         <v>RVND</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I29" s="5">
         <v>50</v>
       </c>
-      <c r="J29" s="6">
-        <v>10809.47</v>
-      </c>
-      <c r="K29" s="9">
+      <c r="J29" s="9">
+        <v>9949.44</v>
+      </c>
+      <c r="K29" s="6">
         <v>10075.59</v>
       </c>
       <c r="L29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="O29" s="11">
+        <v>32</v>
+      </c>
+      <c r="O29" s="10">
         <v>75</v>
       </c>
-      <c r="P29" s="12">
-        <v>15643.09</v>
-      </c>
-      <c r="Q29" s="9">
+      <c r="P29" s="9">
+        <v>15214.86</v>
+      </c>
+      <c r="Q29" s="6">
         <v>14544.38</v>
       </c>
-      <c r="R29" s="13" t="str">
+      <c r="R29" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="30" ht="15.75" spans="2:18">
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" s="5">
         <v>37</v>
       </c>
       <c r="D30" s="6">
-        <v>6476.43</v>
+        <v>6400.64</v>
       </c>
       <c r="E30" s="7">
         <v>6400.64</v>
       </c>
       <c r="F30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I30" s="5">
         <v>75</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="9">
         <v>13750.65</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="6">
         <v>14013.34</v>
       </c>
       <c r="L30" s="4" t="str">
@@ -2691,25 +2682,25 @@
         <v>RVND2</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O30" s="11">
+        <v>33</v>
+      </c>
+      <c r="O30" s="10">
         <v>112</v>
       </c>
-      <c r="P30" s="12">
-        <v>20322.55</v>
-      </c>
-      <c r="Q30" s="9">
+      <c r="P30" s="9">
+        <v>19416.42</v>
+      </c>
+      <c r="Q30" s="6">
         <v>19944.47</v>
       </c>
-      <c r="R30" s="13" t="str">
+      <c r="R30" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="2:18">
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31" s="5">
         <v>50</v>
@@ -2725,15 +2716,15 @@
         <v>Igual</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I31" s="5">
         <v>100</v>
       </c>
-      <c r="J31" s="6">
-        <v>13485.45</v>
-      </c>
-      <c r="K31" s="9">
+      <c r="J31" s="9">
+        <v>13325.47</v>
+      </c>
+      <c r="K31" s="6">
         <v>12922.46</v>
       </c>
       <c r="L31" s="4" t="str">
@@ -2741,49 +2732,49 @@
         <v>RVND</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O31" s="11">
+        <v>34</v>
+      </c>
+      <c r="O31" s="10">
         <v>150</v>
       </c>
-      <c r="P31" s="12">
-        <v>20771</v>
-      </c>
-      <c r="Q31" s="9">
+      <c r="P31" s="9">
+        <v>20638.75</v>
+      </c>
+      <c r="Q31" s="6">
         <v>20463.14</v>
       </c>
-      <c r="R31" s="13" t="str">
+      <c r="R31" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="2:18">
       <c r="B32" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" s="5">
         <v>25</v>
       </c>
       <c r="D32" s="6">
-        <v>5507.89</v>
+        <v>5393.56</v>
       </c>
       <c r="E32" s="7">
         <v>5393.56</v>
       </c>
       <c r="F32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I32" s="5">
         <v>50</v>
       </c>
-      <c r="J32" s="6">
-        <v>11184.6</v>
-      </c>
-      <c r="K32" s="9">
+      <c r="J32" s="9">
+        <v>10851.38</v>
+      </c>
+      <c r="K32" s="6">
         <v>10708.33</v>
       </c>
       <c r="L32" s="4" t="str">
@@ -2791,31 +2782,31 @@
         <v>RVND</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="O32" s="11">
+        <v>35</v>
+      </c>
+      <c r="O32" s="10">
         <v>75</v>
       </c>
-      <c r="P32" s="12">
-        <v>16884.09</v>
-      </c>
-      <c r="Q32" s="9">
+      <c r="P32" s="9">
+        <v>15957.25</v>
+      </c>
+      <c r="Q32" s="6">
         <v>15454.66</v>
       </c>
-      <c r="R32" s="13" t="str">
+      <c r="R32" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="2:18">
       <c r="B33" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C33" s="5">
         <v>37</v>
       </c>
       <c r="D33" s="6">
-        <v>5119.54</v>
+        <v>5053.72</v>
       </c>
       <c r="E33" s="7">
         <v>5003.2</v>
@@ -2825,15 +2816,15 @@
         <v>RVND</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I33" s="5">
         <v>75</v>
       </c>
-      <c r="J33" s="6">
-        <v>11814.94</v>
-      </c>
-      <c r="K33" s="9">
+      <c r="J33" s="9">
+        <v>11203.48</v>
+      </c>
+      <c r="K33" s="6">
         <v>11076.35</v>
       </c>
       <c r="L33" s="4" t="str">
@@ -2841,31 +2832,31 @@
         <v>RVND</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="O33" s="11">
+        <v>36</v>
+      </c>
+      <c r="O33" s="10">
         <v>112</v>
       </c>
-      <c r="P33" s="12">
-        <v>17109.45</v>
-      </c>
-      <c r="Q33" s="9">
+      <c r="P33" s="9">
+        <v>17011.55</v>
+      </c>
+      <c r="Q33" s="6">
         <v>16688.08</v>
       </c>
-      <c r="R33" s="13" t="str">
+      <c r="R33" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="2:18">
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5">
         <v>50</v>
       </c>
       <c r="D34" s="6">
-        <v>6789.91</v>
+        <v>6486.19</v>
       </c>
       <c r="E34" s="7">
         <v>6359.99</v>
@@ -2875,15 +2866,15 @@
         <v>RVND</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I34" s="5">
         <v>100</v>
       </c>
-      <c r="J34" s="6">
-        <v>15448.82</v>
-      </c>
-      <c r="K34" s="9">
+      <c r="J34" s="9">
+        <v>14530.78</v>
+      </c>
+      <c r="K34" s="6">
         <v>14033.62</v>
       </c>
       <c r="L34" s="4" t="str">
@@ -2891,31 +2882,31 @@
         <v>RVND</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="O34" s="11">
+        <v>37</v>
+      </c>
+      <c r="O34" s="10">
         <v>150</v>
       </c>
-      <c r="P34" s="12">
-        <v>21809.73</v>
-      </c>
-      <c r="Q34" s="9">
+      <c r="P34" s="9">
+        <v>20691.31</v>
+      </c>
+      <c r="Q34" s="6">
         <v>20173.58</v>
       </c>
-      <c r="R34" s="13" t="str">
+      <c r="R34" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="35" ht="15.75" spans="2:18">
       <c r="B35" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="5">
         <v>25</v>
       </c>
       <c r="D35" s="6">
-        <v>4293.02</v>
+        <v>4275.81</v>
       </c>
       <c r="E35" s="7">
         <v>4236.4</v>
@@ -2925,15 +2916,15 @@
         <v>RVND</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I35" s="5">
         <v>50</v>
       </c>
-      <c r="J35" s="6">
-        <v>9555.73</v>
-      </c>
-      <c r="K35" s="9">
+      <c r="J35" s="9">
+        <v>8884.33</v>
+      </c>
+      <c r="K35" s="6">
         <v>8632.68</v>
       </c>
       <c r="L35" s="4" t="str">
@@ -2941,99 +2932,99 @@
         <v>RVND</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="O35" s="11">
+        <v>38</v>
+      </c>
+      <c r="O35" s="10">
         <v>75</v>
       </c>
-      <c r="P35" s="12">
-        <v>14209.95</v>
-      </c>
-      <c r="Q35" s="9">
+      <c r="P35" s="9">
+        <v>14413.28</v>
+      </c>
+      <c r="Q35" s="6">
         <v>13951.85</v>
       </c>
-      <c r="R35" s="13" t="str">
+      <c r="R35" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="2:18">
       <c r="B36" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="5">
         <v>25</v>
       </c>
       <c r="D36" s="6">
-        <v>5155.74</v>
+        <v>5235.81</v>
       </c>
       <c r="E36" s="7">
         <v>5220.64</v>
       </c>
       <c r="F36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>RVND2</v>
+        <v>RVND</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I36" s="5">
         <v>50</v>
       </c>
-      <c r="J36" s="6">
-        <v>10205.07</v>
-      </c>
-      <c r="K36" s="9">
+      <c r="J36" s="9">
+        <v>10204.13</v>
+      </c>
+      <c r="K36" s="6">
         <v>10204.13</v>
       </c>
       <c r="L36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="O36" s="11">
+        <v>39</v>
+      </c>
+      <c r="O36" s="10">
         <v>75</v>
       </c>
-      <c r="P36" s="12">
-        <v>14992.79</v>
-      </c>
-      <c r="Q36" s="9">
+      <c r="P36" s="9">
+        <v>14991.85</v>
+      </c>
+      <c r="Q36" s="6">
         <v>14779.43</v>
       </c>
-      <c r="R36" s="13" t="str">
+      <c r="R36" s="11" t="str">
         <f t="shared" si="2"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="2:18">
       <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" s="5">
         <v>25</v>
       </c>
       <c r="D37" s="6">
-        <v>4059.43</v>
+        <v>3894.47</v>
       </c>
       <c r="E37" s="7">
         <v>3894.47</v>
       </c>
       <c r="F37" s="4" t="str">
         <f t="shared" ref="F37:F65" si="3">IF(D37&lt;E37,"RVND2",IF(E37&lt;D37,"RVND","Igual"))</f>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I37" s="5">
         <v>50</v>
       </c>
-      <c r="J37" s="6">
-        <v>9424.1</v>
-      </c>
-      <c r="K37" s="9">
+      <c r="J37" s="9">
+        <v>9310.42</v>
+      </c>
+      <c r="K37" s="6">
         <v>9060.14</v>
       </c>
       <c r="L37" s="4" t="str">
@@ -3041,31 +3032,31 @@
         <v>RVND</v>
       </c>
       <c r="N37" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="O37" s="11">
+        <v>40</v>
+      </c>
+      <c r="O37" s="10">
         <v>75</v>
       </c>
-      <c r="P37" s="12">
-        <v>15400.35</v>
-      </c>
-      <c r="Q37" s="9">
+      <c r="P37" s="9">
+        <v>15286.66</v>
+      </c>
+      <c r="Q37" s="6">
         <v>14943.31</v>
       </c>
-      <c r="R37" s="13" t="str">
+      <c r="R37" s="11" t="str">
         <f t="shared" ref="R37:R65" si="5">IF(P37&lt;Q37,"RVND2",IF(Q37&lt;P37,"RVND","Igual"))</f>
         <v>RVND</v>
       </c>
     </row>
     <row r="38" ht="15.75" spans="2:18">
       <c r="B38" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="5">
         <v>26</v>
       </c>
       <c r="D38" s="6">
-        <v>2108.36</v>
+        <v>2043.71</v>
       </c>
       <c r="E38" s="7">
         <v>2002.98</v>
@@ -3075,47 +3066,47 @@
         <v>RVND</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I38" s="5">
         <v>52</v>
       </c>
-      <c r="J38" s="6">
-        <v>5532.5</v>
-      </c>
-      <c r="K38" s="9">
+      <c r="J38" s="9">
+        <v>5398.45</v>
+      </c>
+      <c r="K38" s="6">
         <v>5425.48</v>
       </c>
       <c r="L38" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="O38" s="11">
+        <v>41</v>
+      </c>
+      <c r="O38" s="10">
         <v>78</v>
       </c>
-      <c r="P38" s="12">
-        <v>8630.64</v>
-      </c>
-      <c r="Q38" s="9">
+      <c r="P38" s="9">
         <v>8397.36</v>
       </c>
-      <c r="R38" s="13" t="str">
+      <c r="Q38" s="6">
+        <v>8397.36</v>
+      </c>
+      <c r="R38" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="39" ht="15.75" spans="2:18">
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="5">
         <v>79</v>
       </c>
       <c r="D39" s="6">
-        <v>8705.92</v>
+        <v>8598.9</v>
       </c>
       <c r="E39" s="7">
         <v>8571.87</v>
@@ -3125,15 +3116,15 @@
         <v>RVND</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I39" s="5">
         <v>159</v>
       </c>
-      <c r="J39" s="6">
-        <v>20575.41</v>
-      </c>
-      <c r="K39" s="9">
+      <c r="J39" s="9">
+        <v>19200.56</v>
+      </c>
+      <c r="K39" s="6">
         <v>18685.55</v>
       </c>
       <c r="L39" s="4" t="str">
@@ -3141,31 +3132,31 @@
         <v>RVND</v>
       </c>
       <c r="N39" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O39" s="11">
+        <v>42</v>
+      </c>
+      <c r="O39" s="10">
         <v>238</v>
       </c>
-      <c r="P39" s="12">
-        <v>30020.55</v>
-      </c>
-      <c r="Q39" s="9">
+      <c r="P39" s="9">
+        <v>28509.77</v>
+      </c>
+      <c r="Q39" s="6">
         <v>28655.37</v>
       </c>
-      <c r="R39" s="13" t="str">
+      <c r="R39" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="40" ht="15.75" spans="2:18">
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40" s="5">
         <v>344</v>
       </c>
       <c r="D40" s="6">
-        <v>12973.05</v>
+        <v>12751.26</v>
       </c>
       <c r="E40" s="7">
         <v>12540.17</v>
@@ -3175,15 +3166,15 @@
         <v>RVND</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I40" s="5">
         <v>689</v>
       </c>
-      <c r="J40" s="6">
-        <v>27832.69</v>
-      </c>
-      <c r="K40" s="9">
+      <c r="J40" s="9">
+        <v>27349.8</v>
+      </c>
+      <c r="K40" s="6">
         <v>26839.14</v>
       </c>
       <c r="L40" s="4" t="str">
@@ -3191,31 +3182,30 @@
         <v>RVND</v>
       </c>
       <c r="N40" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="O40" s="11">
+        <v>43</v>
+      </c>
+      <c r="O40" s="10">
         <v>1034</v>
       </c>
-      <c r="P40" s="12">
-        <v>44054.85</v>
-      </c>
-      <c r="Q40" s="9">
+      <c r="P40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" s="6">
         <v>42522.62</v>
       </c>
-      <c r="R40" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R40" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="41" ht="15.75" spans="2:18">
       <c r="B41" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41" s="5">
         <v>140</v>
       </c>
       <c r="D41" s="6">
-        <v>712</v>
+        <v>672</v>
       </c>
       <c r="E41" s="7">
         <v>670</v>
@@ -3225,47 +3215,46 @@
         <v>RVND</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I41" s="5">
         <v>280</v>
       </c>
-      <c r="J41" s="6">
-        <v>1319</v>
-      </c>
-      <c r="K41" s="9">
+      <c r="J41" s="9">
+        <v>1228</v>
+      </c>
+      <c r="K41" s="6">
         <v>1236</v>
       </c>
       <c r="L41" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="O41" s="11">
+        <v>44</v>
+      </c>
+      <c r="O41" s="10">
         <v>420</v>
       </c>
-      <c r="P41" s="12">
-        <v>2166</v>
-      </c>
-      <c r="Q41" s="9">
+      <c r="P41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="6">
         <v>2028</v>
       </c>
-      <c r="R41" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R41" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="42" ht="15.75" spans="2:18">
       <c r="B42" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C42" s="5">
         <v>19</v>
       </c>
       <c r="D42" s="6">
-        <v>25126.84</v>
+        <v>23567.43</v>
       </c>
       <c r="E42" s="7">
         <v>21496.25</v>
@@ -3275,15 +3264,15 @@
         <v>RVND</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I42" s="5">
         <v>38</v>
       </c>
-      <c r="J42" s="6">
-        <v>42676.77</v>
-      </c>
-      <c r="K42" s="9">
+      <c r="J42" s="9">
+        <v>42305.92</v>
+      </c>
+      <c r="K42" s="6">
         <v>42006.67</v>
       </c>
       <c r="L42" s="4" t="str">
@@ -3291,31 +3280,31 @@
         <v>RVND</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O42" s="11">
+        <v>45</v>
+      </c>
+      <c r="O42" s="10">
         <v>57</v>
       </c>
-      <c r="P42" s="12">
-        <v>62054.84</v>
-      </c>
-      <c r="Q42" s="9">
+      <c r="P42" s="9">
+        <v>60179.48</v>
+      </c>
+      <c r="Q42" s="6">
         <v>61124.81</v>
       </c>
-      <c r="R42" s="13" t="str">
+      <c r="R42" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="43" ht="15.75" spans="2:18">
       <c r="B43" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" s="5">
         <v>26</v>
       </c>
       <c r="D43" s="6">
-        <v>7304.83</v>
+        <v>7222.71</v>
       </c>
       <c r="E43" s="7">
         <v>7038.06</v>
@@ -3325,65 +3314,65 @@
         <v>RVND</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I43" s="5">
         <v>52</v>
       </c>
-      <c r="J43" s="6">
-        <v>15175.12</v>
-      </c>
-      <c r="K43" s="9">
+      <c r="J43" s="9">
+        <v>15092.28</v>
+      </c>
+      <c r="K43" s="6">
         <v>15092.28</v>
       </c>
       <c r="L43" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O43" s="11">
+        <v>46</v>
+      </c>
+      <c r="O43" s="10">
         <v>80</v>
       </c>
-      <c r="P43" s="12">
-        <v>30283.4</v>
-      </c>
-      <c r="Q43" s="9">
+      <c r="P43" s="9">
+        <v>30115.85</v>
+      </c>
+      <c r="Q43" s="6">
         <v>30429.58</v>
       </c>
-      <c r="R43" s="13" t="str">
+      <c r="R43" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND2</v>
       </c>
     </row>
     <row r="44" ht="15.75" spans="2:18">
       <c r="B44" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44" s="5">
         <v>31</v>
       </c>
       <c r="D44" s="6">
-        <v>10765.78</v>
+        <v>10080.05</v>
       </c>
       <c r="E44" s="7">
         <v>10080.05</v>
       </c>
       <c r="F44" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I44" s="5">
         <v>62</v>
       </c>
-      <c r="J44" s="6">
-        <v>22804.99</v>
-      </c>
-      <c r="K44" s="9">
+      <c r="J44" s="9">
+        <v>22476.1</v>
+      </c>
+      <c r="K44" s="6">
         <v>22935.61</v>
       </c>
       <c r="L44" s="4" t="str">
@@ -3391,75 +3380,75 @@
         <v>RVND2</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="O44" s="11">
+        <v>47</v>
+      </c>
+      <c r="O44" s="10">
         <v>93</v>
       </c>
-      <c r="P44" s="12">
-        <v>37699.23</v>
-      </c>
-      <c r="Q44" s="9">
+      <c r="P44" s="9">
+        <v>36899.68</v>
+      </c>
+      <c r="Q44" s="6">
         <v>36650.4</v>
       </c>
-      <c r="R44" s="13" t="str">
+      <c r="R44" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="2:18">
       <c r="B45" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C45" s="5">
         <v>34</v>
       </c>
       <c r="D45" s="6">
-        <v>21167.89</v>
+        <v>20642.54</v>
       </c>
       <c r="E45" s="7">
         <v>20714.89</v>
       </c>
       <c r="F45" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I45" s="5">
         <v>68</v>
       </c>
-      <c r="J45" s="6">
-        <v>45314.79</v>
-      </c>
-      <c r="K45" s="9">
+      <c r="J45" s="9">
+        <v>45462.43</v>
+      </c>
+      <c r="K45" s="6">
         <v>45462.43</v>
       </c>
       <c r="L45" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND2</v>
+        <v>Igual</v>
       </c>
       <c r="N45" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O45" s="11">
+        <v>48</v>
+      </c>
+      <c r="O45" s="10">
         <v>102</v>
       </c>
-      <c r="P45" s="12">
-        <v>74400.9</v>
-      </c>
-      <c r="Q45" s="9">
+      <c r="P45" s="9">
+        <v>72330.48</v>
+      </c>
+      <c r="Q45" s="6">
         <v>68368.27</v>
       </c>
-      <c r="R45" s="13" t="str">
+      <c r="R45" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="2:18">
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46" s="5">
         <v>36</v>
@@ -3475,15 +3464,15 @@
         <v>Igual</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I46" s="5">
         <v>72</v>
       </c>
-      <c r="J46" s="6">
-        <v>26295.98</v>
-      </c>
-      <c r="K46" s="9">
+      <c r="J46" s="9">
+        <v>26035.91</v>
+      </c>
+      <c r="K46" s="6">
         <v>25880.31</v>
       </c>
       <c r="L46" s="4" t="str">
@@ -3491,99 +3480,99 @@
         <v>RVND</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="O46" s="11">
+        <v>49</v>
+      </c>
+      <c r="O46" s="10">
         <v>108</v>
       </c>
-      <c r="P46" s="12">
-        <v>40832.2</v>
-      </c>
-      <c r="Q46" s="9">
+      <c r="P46" s="9">
+        <v>40287.04</v>
+      </c>
+      <c r="Q46" s="6">
         <v>40210.94</v>
       </c>
-      <c r="R46" s="13" t="str">
+      <c r="R46" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="2:18">
       <c r="B47" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47" s="5">
         <v>38</v>
       </c>
       <c r="D47" s="6">
-        <v>15403.26</v>
+        <v>14780.62</v>
       </c>
       <c r="E47" s="7">
         <v>14780.62</v>
       </c>
       <c r="F47" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I47" s="5">
         <v>76</v>
       </c>
-      <c r="J47" s="6">
-        <v>32745.67</v>
-      </c>
-      <c r="K47" s="9">
+      <c r="J47" s="9">
+        <v>32440.64</v>
+      </c>
+      <c r="K47" s="6">
         <v>32440.64</v>
       </c>
       <c r="L47" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="N47" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O47" s="11">
+        <v>50</v>
+      </c>
+      <c r="O47" s="10">
         <v>114</v>
       </c>
-      <c r="P47" s="12">
-        <v>46419.17</v>
-      </c>
-      <c r="Q47" s="9">
+      <c r="P47" s="9">
         <v>46089.98</v>
       </c>
-      <c r="R47" s="13" t="str">
+      <c r="Q47" s="6">
+        <v>46089.98</v>
+      </c>
+      <c r="R47" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="48" ht="15.75" spans="2:18">
       <c r="B48" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48" s="5">
         <v>56</v>
       </c>
       <c r="D48" s="6">
-        <v>21631.43</v>
+        <v>21374.46</v>
       </c>
       <c r="E48" s="7">
         <v>21374.46</v>
       </c>
       <c r="F48" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I48" s="5">
         <v>113</v>
       </c>
-      <c r="J48" s="6">
-        <v>46356.13</v>
-      </c>
-      <c r="K48" s="9">
+      <c r="J48" s="9">
+        <v>41305.91</v>
+      </c>
+      <c r="K48" s="6">
         <v>41301.91</v>
       </c>
       <c r="L48" s="4" t="str">
@@ -3591,31 +3580,31 @@
         <v>RVND</v>
       </c>
       <c r="N48" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="O48" s="11">
+        <v>51</v>
+      </c>
+      <c r="O48" s="10">
         <v>169</v>
       </c>
-      <c r="P48" s="12">
-        <v>61912.01</v>
-      </c>
-      <c r="Q48" s="9">
+      <c r="P48" s="9">
+        <v>46590.52</v>
+      </c>
+      <c r="Q48" s="6">
         <v>48188.7</v>
       </c>
-      <c r="R48" s="13" t="str">
+      <c r="R48" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="49" ht="15.75" spans="2:18">
       <c r="B49" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49" s="5">
         <v>66</v>
       </c>
       <c r="D49" s="6">
-        <v>8023.61</v>
+        <v>7916.23</v>
       </c>
       <c r="E49" s="7">
         <v>7800</v>
@@ -3625,15 +3614,15 @@
         <v>RVND</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I49" s="5">
         <v>132</v>
       </c>
-      <c r="J49" s="6">
+      <c r="J49" s="9">
         <v>21568.72</v>
       </c>
-      <c r="K49" s="9">
+      <c r="K49" s="6">
         <v>21568.72</v>
       </c>
       <c r="L49" s="4" t="str">
@@ -3641,31 +3630,31 @@
         <v>Igual</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="O49" s="11">
+        <v>52</v>
+      </c>
+      <c r="O49" s="10">
         <v>198</v>
       </c>
-      <c r="P49" s="12">
-        <v>35315.89</v>
-      </c>
-      <c r="Q49" s="9">
+      <c r="P49" s="9">
+        <v>34348.07</v>
+      </c>
+      <c r="Q49" s="6">
         <v>33880.01</v>
       </c>
-      <c r="R49" s="13" t="str">
+      <c r="R49" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="50" ht="15.75" spans="2:18">
       <c r="B50" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50" s="5">
         <v>74</v>
       </c>
       <c r="D50" s="6">
-        <v>11960.02</v>
+        <v>11124.49</v>
       </c>
       <c r="E50" s="7">
         <v>10579.89</v>
@@ -3675,65 +3664,65 @@
         <v>RVND</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I50" s="5">
         <v>149</v>
       </c>
-      <c r="J50" s="6">
-        <v>24745.62</v>
-      </c>
-      <c r="K50" s="9">
+      <c r="J50" s="9">
+        <v>23514.28</v>
+      </c>
+      <c r="K50" s="6">
         <v>23845.29</v>
       </c>
       <c r="L50" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="O50" s="11">
+        <v>53</v>
+      </c>
+      <c r="O50" s="10">
         <v>224</v>
       </c>
-      <c r="P50" s="12">
-        <v>35840.67</v>
-      </c>
-      <c r="Q50" s="9">
+      <c r="P50" s="9">
+        <v>34767.41</v>
+      </c>
+      <c r="Q50" s="6">
         <v>34501.38</v>
       </c>
-      <c r="R50" s="13" t="str">
+      <c r="R50" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="51" ht="15.75" spans="2:18">
       <c r="B51" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51" s="5">
         <v>109</v>
       </c>
       <c r="D51" s="6">
-        <v>21579.24</v>
+        <v>19864.15</v>
       </c>
       <c r="E51" s="7">
         <v>19972.3</v>
       </c>
       <c r="F51" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I51" s="5">
         <v>219</v>
       </c>
-      <c r="J51" s="6">
-        <v>39638.84</v>
-      </c>
-      <c r="K51" s="9">
+      <c r="J51" s="9">
+        <v>38397.87</v>
+      </c>
+      <c r="K51" s="6">
         <v>36727.88</v>
       </c>
       <c r="L51" s="4" t="str">
@@ -3741,31 +3730,31 @@
         <v>RVND</v>
       </c>
       <c r="N51" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="O51" s="11">
+        <v>54</v>
+      </c>
+      <c r="O51" s="10">
         <v>329</v>
       </c>
-      <c r="P51" s="12">
-        <v>63250.26</v>
-      </c>
-      <c r="Q51" s="9">
+      <c r="P51" s="9">
+        <v>62198.91</v>
+      </c>
+      <c r="Q51" s="6">
         <v>61894.86</v>
       </c>
-      <c r="R51" s="13" t="str">
+      <c r="R51" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="52" ht="15.75" spans="2:18">
       <c r="B52" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C52" s="5">
         <v>250</v>
       </c>
       <c r="D52" s="6">
-        <v>65639.35</v>
+        <v>62104.52</v>
       </c>
       <c r="E52" s="7">
         <v>58420.15</v>
@@ -3775,15 +3764,15 @@
         <v>RVND</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I52" s="5">
         <v>501</v>
       </c>
-      <c r="J52" s="6">
-        <v>126529.13</v>
-      </c>
-      <c r="K52" s="9">
+      <c r="J52" s="9">
+        <v>123303.19</v>
+      </c>
+      <c r="K52" s="6">
         <v>117296.16</v>
       </c>
       <c r="L52" s="4" t="str">
@@ -3791,49 +3780,48 @@
         <v>RVND</v>
       </c>
       <c r="N52" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O52" s="11">
+        <v>55</v>
+      </c>
+      <c r="O52" s="10">
         <v>751</v>
       </c>
-      <c r="P52" s="12">
-        <v>193932.93</v>
-      </c>
-      <c r="Q52" s="9">
+      <c r="P52" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q52" s="6">
         <v>184532.11</v>
       </c>
-      <c r="R52" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R52" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="53" ht="15.75" spans="2:18">
       <c r="B53" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C53" s="5">
         <v>24</v>
       </c>
       <c r="D53" s="6">
-        <v>263.3</v>
+        <v>255.03</v>
       </c>
       <c r="E53" s="7">
         <v>255.03</v>
       </c>
       <c r="F53" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I53" s="5">
         <v>49</v>
       </c>
-      <c r="J53" s="6">
-        <v>560.12</v>
-      </c>
-      <c r="K53" s="9">
+      <c r="J53" s="9">
+        <v>571.86</v>
+      </c>
+      <c r="K53" s="6">
         <v>557.86</v>
       </c>
       <c r="L53" s="4" t="str">
@@ -3841,49 +3829,49 @@
         <v>RVND</v>
       </c>
       <c r="N53" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="O53" s="11">
+        <v>56</v>
+      </c>
+      <c r="O53" s="10">
         <v>74</v>
       </c>
-      <c r="P53" s="12">
-        <v>889.04</v>
-      </c>
-      <c r="Q53" s="9">
+      <c r="P53" s="9">
+        <v>861.9</v>
+      </c>
+      <c r="Q53" s="6">
         <v>864.95</v>
       </c>
-      <c r="R53" s="13" t="str">
+      <c r="R53" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="54" ht="15.75" spans="2:18">
       <c r="B54" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C54" s="5">
         <v>48</v>
       </c>
       <c r="D54" s="6">
-        <v>538.45</v>
+        <v>529.26</v>
       </c>
       <c r="E54" s="7">
         <v>529.26</v>
       </c>
       <c r="F54" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I54" s="5">
         <v>97</v>
       </c>
-      <c r="J54" s="6">
+      <c r="J54" s="9">
         <v>1109.72</v>
       </c>
-      <c r="K54" s="9">
+      <c r="K54" s="6">
         <v>1109.68</v>
       </c>
       <c r="L54" s="4" t="str">
@@ -3891,31 +3879,31 @@
         <v>RVND</v>
       </c>
       <c r="N54" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="O54" s="11">
+        <v>57</v>
+      </c>
+      <c r="O54" s="10">
         <v>146</v>
       </c>
-      <c r="P54" s="12">
-        <v>1669.95</v>
-      </c>
-      <c r="Q54" s="9">
+      <c r="P54" s="9">
         <v>1669.63</v>
       </c>
-      <c r="R54" s="13" t="str">
+      <c r="Q54" s="6">
+        <v>1669.63</v>
+      </c>
+      <c r="R54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="55" ht="15.75" spans="2:18">
       <c r="B55" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C55" s="5">
         <v>143</v>
       </c>
       <c r="D55" s="6">
-        <v>1665.59</v>
+        <v>1647.9</v>
       </c>
       <c r="E55" s="7">
         <v>1631</v>
@@ -3925,15 +3913,15 @@
         <v>RVND</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I55" s="5">
         <v>287</v>
       </c>
-      <c r="J55" s="6">
-        <v>3343.82</v>
-      </c>
-      <c r="K55" s="9">
+      <c r="J55" s="9">
+        <v>3284.76</v>
+      </c>
+      <c r="K55" s="6">
         <v>3239.8</v>
       </c>
       <c r="L55" s="4" t="str">
@@ -3941,31 +3929,30 @@
         <v>RVND</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="O55" s="11">
+        <v>58</v>
+      </c>
+      <c r="O55" s="10">
         <v>431</v>
       </c>
-      <c r="P55" s="12">
-        <v>5216.35</v>
-      </c>
-      <c r="Q55" s="9">
+      <c r="P55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q55" s="6">
         <v>5042.6</v>
       </c>
-      <c r="R55" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R55" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="56" ht="15.75" spans="2:18">
       <c r="B56" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C56" s="5">
         <v>195</v>
       </c>
       <c r="D56" s="6">
-        <v>2211.2</v>
+        <v>2180.27</v>
       </c>
       <c r="E56" s="7">
         <v>2143.87</v>
@@ -3975,15 +3962,15 @@
         <v>RVND</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I56" s="5">
         <v>391</v>
       </c>
-      <c r="J56" s="6">
-        <v>4406.12</v>
-      </c>
-      <c r="K56" s="9">
+      <c r="J56" s="9">
+        <v>4320.95</v>
+      </c>
+      <c r="K56" s="6">
         <v>4281.01</v>
       </c>
       <c r="L56" s="4" t="str">
@@ -3991,31 +3978,30 @@
         <v>RVND</v>
       </c>
       <c r="N56" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="O56" s="11">
+        <v>59</v>
+      </c>
+      <c r="O56" s="10">
         <v>587</v>
       </c>
-      <c r="P56" s="12">
-        <v>6815.97</v>
-      </c>
-      <c r="Q56" s="9">
+      <c r="P56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" s="6">
         <v>6681.59</v>
       </c>
-      <c r="R56" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R56" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="57" ht="15.75" spans="2:18">
       <c r="B57" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57" s="5">
         <v>43</v>
       </c>
       <c r="D57" s="6">
-        <v>5224</v>
+        <v>5015</v>
       </c>
       <c r="E57" s="7">
         <v>4862</v>
@@ -4025,15 +4011,15 @@
         <v>RVND</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I57" s="5">
         <v>87</v>
       </c>
-      <c r="J57" s="6">
-        <v>10482</v>
-      </c>
-      <c r="K57" s="9">
+      <c r="J57" s="9">
+        <v>10464</v>
+      </c>
+      <c r="K57" s="6">
         <v>10179</v>
       </c>
       <c r="L57" s="4" t="str">
@@ -4041,31 +4027,31 @@
         <v>RVND</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="O57" s="11">
+        <v>60</v>
+      </c>
+      <c r="O57" s="10">
         <v>131</v>
       </c>
-      <c r="P57" s="12">
-        <v>15783</v>
-      </c>
-      <c r="Q57" s="9">
+      <c r="P57" s="9">
+        <v>15707</v>
+      </c>
+      <c r="Q57" s="6">
         <v>15733</v>
       </c>
-      <c r="R57" s="13" t="str">
+      <c r="R57" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>RVND2</v>
       </c>
     </row>
     <row r="58" ht="15.75" spans="2:18">
       <c r="B58" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C58" s="5">
         <v>133</v>
       </c>
       <c r="D58" s="6">
-        <v>12076</v>
+        <v>11894</v>
       </c>
       <c r="E58" s="7">
         <v>11355</v>
@@ -4075,15 +4061,15 @@
         <v>RVND</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I58" s="5">
         <v>267</v>
       </c>
-      <c r="J58" s="6">
-        <v>23147</v>
-      </c>
-      <c r="K58" s="9">
+      <c r="J58" s="9">
+        <v>22775</v>
+      </c>
+      <c r="K58" s="6">
         <v>22763</v>
       </c>
       <c r="L58" s="4" t="str">
@@ -4091,25 +4077,24 @@
         <v>RVND</v>
       </c>
       <c r="N58" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="O58" s="11">
+        <v>61</v>
+      </c>
+      <c r="O58" s="10">
         <v>401</v>
       </c>
-      <c r="P58" s="12">
-        <v>35820</v>
-      </c>
-      <c r="Q58" s="9">
+      <c r="P58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="6">
         <v>35278</v>
       </c>
-      <c r="R58" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R58" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="59" ht="15.75" spans="2:18">
       <c r="B59" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C59" s="5">
         <v>258</v>
@@ -4125,15 +4110,15 @@
         <v>Igual</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I59" s="5">
         <v>516</v>
       </c>
-      <c r="J59" s="6">
-        <v>45854</v>
-      </c>
-      <c r="K59" s="9">
+      <c r="J59" s="9">
+        <v>45986</v>
+      </c>
+      <c r="K59" s="6">
         <v>45504</v>
       </c>
       <c r="L59" s="4" t="str">
@@ -4141,25 +4126,24 @@
         <v>RVND</v>
       </c>
       <c r="N59" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="O59" s="11">
+        <v>62</v>
+      </c>
+      <c r="O59" s="10">
         <v>774</v>
       </c>
-      <c r="P59" s="12">
-        <v>69945</v>
-      </c>
-      <c r="Q59" s="9">
+      <c r="P59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" s="6">
         <v>69819</v>
       </c>
-      <c r="R59" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>RVND</v>
+      <c r="R59" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="60" ht="15.75" spans="2:18">
       <c r="B60" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C60" s="5">
         <v>17</v>
@@ -4175,15 +4159,15 @@
         <v>RVND</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I60" s="5">
         <v>35</v>
       </c>
-      <c r="J60" s="6">
-        <v>308.25</v>
-      </c>
-      <c r="K60" s="9">
+      <c r="J60" s="9">
+        <v>287.1</v>
+      </c>
+      <c r="K60" s="6">
         <v>274.86</v>
       </c>
       <c r="L60" s="4" t="str">
@@ -4191,25 +4175,25 @@
         <v>RVND</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O60" s="11">
+        <v>63</v>
+      </c>
+      <c r="O60" s="10">
         <v>52</v>
       </c>
-      <c r="P60" s="12">
-        <v>476.47</v>
-      </c>
-      <c r="Q60" s="9">
+      <c r="P60" s="9">
+        <v>442.37</v>
+      </c>
+      <c r="Q60" s="6">
         <v>440.64</v>
       </c>
-      <c r="R60" s="13" t="str">
+      <c r="R60" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="61" ht="15.75" spans="2:18">
       <c r="B61" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C61" s="5">
         <v>10</v>
@@ -4225,15 +4209,15 @@
         <v>Igual</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I61" s="5">
         <v>21</v>
       </c>
-      <c r="J61" s="6">
+      <c r="J61" s="9">
         <v>425</v>
       </c>
-      <c r="K61" s="9">
+      <c r="K61" s="6">
         <v>425</v>
       </c>
       <c r="L61" s="4" t="str">
@@ -4241,25 +4225,25 @@
         <v>Igual</v>
       </c>
       <c r="N61" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="O61" s="11">
+        <v>64</v>
+      </c>
+      <c r="O61" s="10">
         <v>31</v>
       </c>
-      <c r="P61" s="12">
-        <v>720</v>
-      </c>
-      <c r="Q61" s="9">
+      <c r="P61" s="9">
         <v>715</v>
       </c>
-      <c r="R61" s="13" t="str">
+      <c r="Q61" s="6">
+        <v>715</v>
+      </c>
+      <c r="R61" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>RVND</v>
+        <v>Igual</v>
       </c>
     </row>
     <row r="62" ht="15.75" spans="2:18">
       <c r="B62" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C62" s="5">
         <v>56</v>
@@ -4275,15 +4259,15 @@
         <v>Igual</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I62" s="5">
         <v>112</v>
       </c>
-      <c r="J62" s="6">
+      <c r="J62" s="9">
         <v>55500</v>
       </c>
-      <c r="K62" s="9">
+      <c r="K62" s="6">
         <v>55500</v>
       </c>
       <c r="L62" s="4" t="str">
@@ -4291,31 +4275,31 @@
         <v>Igual</v>
       </c>
       <c r="N62" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="O62" s="11">
+        <v>65</v>
+      </c>
+      <c r="O62" s="10">
         <v>168</v>
       </c>
-      <c r="P62" s="12">
-        <v>86863.96</v>
-      </c>
-      <c r="Q62" s="9">
+      <c r="P62" s="9">
+        <v>85778.17</v>
+      </c>
+      <c r="Q62" s="6">
         <v>85571.07</v>
       </c>
-      <c r="R62" s="13" t="str">
+      <c r="R62" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="63" ht="15.75" spans="2:18">
       <c r="B63" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C63" s="5">
         <v>56</v>
       </c>
       <c r="D63" s="6">
-        <v>964.26</v>
+        <v>955.08</v>
       </c>
       <c r="E63" s="7">
         <v>895.66</v>
@@ -4325,15 +4309,15 @@
         <v>RVND</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I63" s="5">
         <v>112</v>
       </c>
-      <c r="J63" s="6">
-        <v>1803.89</v>
-      </c>
-      <c r="K63" s="9">
+      <c r="J63" s="9">
+        <v>1794.71</v>
+      </c>
+      <c r="K63" s="6">
         <v>1760.09</v>
       </c>
       <c r="L63" s="4" t="str">
@@ -4341,25 +4325,25 @@
         <v>RVND</v>
       </c>
       <c r="N63" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O63" s="11">
+        <v>66</v>
+      </c>
+      <c r="O63" s="10">
         <v>168</v>
       </c>
-      <c r="P63" s="12">
-        <v>2685.22</v>
-      </c>
-      <c r="Q63" s="9">
+      <c r="P63" s="9">
+        <v>2620.28</v>
+      </c>
+      <c r="Q63" s="6">
         <v>2614.58</v>
       </c>
-      <c r="R63" s="13" t="str">
+      <c r="R63" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="64" ht="15.75" spans="2:18">
       <c r="B64" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C64" s="5">
         <v>4</v>
@@ -4375,15 +4359,15 @@
         <v>RVND</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I64" s="5">
         <v>8</v>
       </c>
-      <c r="J64" s="6">
+      <c r="J64" s="9">
         <v>1981.71</v>
       </c>
-      <c r="K64" s="9">
+      <c r="K64" s="6">
         <v>1981.71</v>
       </c>
       <c r="L64" s="4" t="str">
@@ -4391,25 +4375,25 @@
         <v>Igual</v>
       </c>
       <c r="N64" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="O64" s="11">
+        <v>67</v>
+      </c>
+      <c r="O64" s="10">
         <v>12</v>
       </c>
-      <c r="P64" s="12">
+      <c r="P64" s="9">
         <v>2741.1</v>
       </c>
-      <c r="Q64" s="9">
+      <c r="Q64" s="6">
         <v>2741.1</v>
       </c>
-      <c r="R64" s="13" t="str">
+      <c r="R64" s="11" t="str">
         <f t="shared" si="5"/>
         <v>Igual</v>
       </c>
     </row>
     <row r="65" ht="15.75" spans="2:18">
       <c r="B65" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C65" s="5">
         <v>5</v>
@@ -4425,15 +4409,15 @@
         <v>Igual</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I65" s="5">
         <v>11</v>
       </c>
-      <c r="J65" s="6">
+      <c r="J65" s="9">
         <v>2062.92</v>
       </c>
-      <c r="K65" s="9">
+      <c r="K65" s="6">
         <v>2062.92</v>
       </c>
       <c r="L65" s="4" t="str">
@@ -4441,52 +4425,52 @@
         <v>Igual</v>
       </c>
       <c r="N65" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O65" s="11">
+        <v>68</v>
+      </c>
+      <c r="O65" s="10">
         <v>16</v>
       </c>
-      <c r="P65" s="12">
-        <v>3049.85</v>
-      </c>
-      <c r="Q65" s="9">
+      <c r="P65" s="9">
+        <v>3025.56</v>
+      </c>
+      <c r="Q65" s="6">
         <v>2540.07</v>
       </c>
-      <c r="R65" s="13" t="str">
+      <c r="R65" s="11" t="str">
         <f t="shared" si="5"/>
         <v>RVND</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="2:4">
       <c r="B69" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" s="1">
         <f>COUNTIF(F4:F65,"RVND")+COUNTIF(L4:L65,"RVND")+COUNTIF(R4:R65,"RVND")</f>
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="C70" s="1">
         <f>COUNTIF(F4:F65,"RVND2")+COUNTIF(L4:L65,"RVND2")+COUNTIF(R4:R65,"RVND2")</f>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D70" s="1">
         <f>COUNTIF(F4:F65,"Igual")+COUNTIF(L4:L65,"Igual")+COUNTIF(R4:R65,"Igual")</f>
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>